<commit_message>
support for importing booleans
</commit_message>
<xml_diff>
--- a/dynamo-spring/src/test/resources/importertest.xlsx
+++ b/dynamo-spring/src/test/resources/importertest.xlsx
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
     <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +433,11 @@
       <c r="F1" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -450,8 +453,11 @@
       <c r="F2" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -470,8 +476,11 @@
       <c r="F3" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -490,8 +499,11 @@
       <c r="F4" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -510,8 +522,11 @@
       <c r="F5" s="2">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -530,8 +545,11 @@
       <c r="F6" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -549,6 +567,9 @@
       </c>
       <c r="F7" s="2">
         <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Date type to import functionality
</commit_message>
<xml_diff>
--- a/dynamo-spring/src/test/resources/importertest.xlsx
+++ b/dynamo-spring/src/test/resources/importertest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,10 +94,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,6 +192,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -226,6 +244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +449,7 @@
     <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +471,11 @@
       <c r="G1" t="b">
         <v>1</v>
       </c>
+      <c r="H1" s="3">
+        <v>41733</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -456,8 +494,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
+      <c r="H2" s="3">
+        <v>42129</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -479,8 +520,9 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -503,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -526,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -549,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
merge from customer branch and big code cleanup
</commit_message>
<xml_diff>
--- a/dynamo-spring/src/test/resources/importertest.xlsx
+++ b/dynamo-spring/src/test/resources/importertest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,10 +94,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,6 +192,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -226,6 +244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +449,7 @@
     <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +471,11 @@
       <c r="G1" t="b">
         <v>1</v>
       </c>
+      <c r="H1" s="3">
+        <v>41733</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -456,8 +494,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
+      <c r="H2" s="3">
+        <v>42129</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -479,8 +520,9 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -503,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -526,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -549,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>

</xml_diff>